<commit_message>
added time to peak effect
</commit_message>
<xml_diff>
--- a/templates/input_data_template.xlsx
+++ b/templates/input_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farah.houdroge\Documents\GitHub\carbomica\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C670D9-B44B-4333-884A-8E8DED652EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E610CFDB-B198-4F22-B409-52B738856A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{0286FA47-14CE-4473-A2C3-5B41DC540DBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="9" xr2:uid="{0286FA47-14CE-4473-A2C3-5B41DC540DBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="10" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="effect sizes" sheetId="6" r:id="rId7"/>
     <sheet name="implementation costs" sheetId="2" r:id="rId8"/>
     <sheet name="maintenance costs" sheetId="11" r:id="rId9"/>
+    <sheet name="time to peak effect" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -209,7 +210,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Specify the total cost for implementing the intervention by facility.
+Specify the total cost for maintaining the intervention by facility.
 The total cost should reflect how much money it would cost to cover the facility 100% with the intervention.</t>
         </r>
       </text>
@@ -218,8 +219,43 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Farah Houdroge</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6D03C8F6-56C7-4D12-A63E-4A59FB9EFFBC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Farah Houdroge:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Specify time to peak effect of intervention (in years, 0 if effect is immediate) as well as how peak effect is reached (gradual or sudden).
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>facilities</t>
   </si>
@@ -435,6 +471,15 @@
   </si>
   <si>
     <t>The first row and column of this table get updated automatically. Specify the total (yearly) cost of maintaining the interventions at full coverage for each facility.</t>
+  </si>
+  <si>
+    <t>Years until peak effect</t>
+  </si>
+  <si>
+    <t>Gradual or sudden onset</t>
+  </si>
+  <si>
+    <t>gradual</t>
   </si>
 </sst>
 </file>
@@ -979,7 +1024,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -995,6 +1040,7 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="43" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1468,6 +1514,1900 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97BDB01-9790-480A-A467-CC2146E6E2C4}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:C309"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="str">
+        <f>IF(interventions!$A2&lt;&gt;"",interventions!$A2,"")</f>
+        <v>intervention_1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="str">
+        <f>IF(interventions!$A3&lt;&gt;"",interventions!$A3,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="str">
+        <f>IF(interventions!$A4&lt;&gt;"",interventions!$A4,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="str">
+        <f>IF(interventions!$A5&lt;&gt;"",interventions!$A5,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="str">
+        <f>IF(interventions!$A6&lt;&gt;"",interventions!$A6,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="str">
+        <f>IF(interventions!$A7&lt;&gt;"",interventions!$A7,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="str">
+        <f>IF(interventions!$A8&lt;&gt;"",interventions!$A8,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="str">
+        <f>IF(interventions!$A9&lt;&gt;"",interventions!$A9,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="str">
+        <f>IF(interventions!$A10&lt;&gt;"",interventions!$A10,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="str">
+        <f>IF(interventions!$A11&lt;&gt;"",interventions!$A11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="str">
+        <f>IF(interventions!$A12&lt;&gt;"",interventions!$A12,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="str">
+        <f>IF(interventions!$A13&lt;&gt;"",interventions!$A13,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="str">
+        <f>IF(interventions!$A14&lt;&gt;"",interventions!$A14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="str">
+        <f>IF(interventions!$A15&lt;&gt;"",interventions!$A15,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="str">
+        <f>IF(interventions!$A16&lt;&gt;"",interventions!$A16,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="str">
+        <f>IF(interventions!$A17&lt;&gt;"",interventions!$A17,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="str">
+        <f>IF(interventions!$A18&lt;&gt;"",interventions!$A18,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="str">
+        <f>IF(interventions!$A19&lt;&gt;"",interventions!$A19,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="str">
+        <f>IF(interventions!$A20&lt;&gt;"",interventions!$A20,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="str">
+        <f>IF(interventions!$A21&lt;&gt;"",interventions!$A21,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="str">
+        <f>IF(interventions!$A22&lt;&gt;"",interventions!$A22,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="str">
+        <f>IF(interventions!$A23&lt;&gt;"",interventions!$A23,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="str">
+        <f>IF(interventions!$A24&lt;&gt;"",interventions!$A24,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="str">
+        <f>IF(interventions!$A25&lt;&gt;"",interventions!$A25,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="str">
+        <f>IF(interventions!$A26&lt;&gt;"",interventions!$A26,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="str">
+        <f>IF(interventions!$A27&lt;&gt;"",interventions!$A27,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="str">
+        <f>IF(interventions!$A28&lt;&gt;"",interventions!$A28,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="str">
+        <f>IF(interventions!$A29&lt;&gt;"",interventions!$A29,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="str">
+        <f>IF(interventions!$A30&lt;&gt;"",interventions!$A30,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="str">
+        <f>IF(interventions!$A31&lt;&gt;"",interventions!$A31,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="str">
+        <f>IF(interventions!$A32&lt;&gt;"",interventions!$A32,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="str">
+        <f>IF(interventions!$A33&lt;&gt;"",interventions!$A33,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="str">
+        <f>IF(interventions!$A34&lt;&gt;"",interventions!$A34,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="str">
+        <f>IF(interventions!$A35&lt;&gt;"",interventions!$A35,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="str">
+        <f>IF(interventions!$A36&lt;&gt;"",interventions!$A36,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="str">
+        <f>IF(interventions!$A37&lt;&gt;"",interventions!$A37,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="str">
+        <f>IF(interventions!$A38&lt;&gt;"",interventions!$A38,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="str">
+        <f>IF(interventions!$A39&lt;&gt;"",interventions!$A39,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="str">
+        <f>IF(interventions!$A40&lt;&gt;"",interventions!$A40,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="str">
+        <f>IF(interventions!$A41&lt;&gt;"",interventions!$A41,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="str">
+        <f>IF(interventions!$A42&lt;&gt;"",interventions!$A42,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="str">
+        <f>IF(interventions!$A43&lt;&gt;"",interventions!$A43,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="str">
+        <f>IF(interventions!$A44&lt;&gt;"",interventions!$A44,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="str">
+        <f>IF(interventions!$A45&lt;&gt;"",interventions!$A45,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="str">
+        <f>IF(interventions!$A46&lt;&gt;"",interventions!$A46,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="str">
+        <f>IF(interventions!$A47&lt;&gt;"",interventions!$A47,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="str">
+        <f>IF(interventions!$A48&lt;&gt;"",interventions!$A48,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="str">
+        <f>IF(interventions!$A49&lt;&gt;"",interventions!$A49,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="str">
+        <f>IF(interventions!$A50&lt;&gt;"",interventions!$A50,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="str">
+        <f>IF(interventions!$A51&lt;&gt;"",interventions!$A51,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="str">
+        <f>IF(interventions!$A52&lt;&gt;"",interventions!$A52,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="str">
+        <f>IF(interventions!$A53&lt;&gt;"",interventions!$A53,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="str">
+        <f>IF(interventions!$A54&lt;&gt;"",interventions!$A54,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="str">
+        <f>IF(interventions!$A55&lt;&gt;"",interventions!$A55,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="str">
+        <f>IF(interventions!$A56&lt;&gt;"",interventions!$A56,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="str">
+        <f>IF(interventions!$A57&lt;&gt;"",interventions!$A57,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="str">
+        <f>IF(interventions!$A58&lt;&gt;"",interventions!$A58,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="str">
+        <f>IF(interventions!$A59&lt;&gt;"",interventions!$A59,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="str">
+        <f>IF(interventions!$A60&lt;&gt;"",interventions!$A60,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="str">
+        <f>IF(interventions!$A61&lt;&gt;"",interventions!$A61,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="str">
+        <f>IF(interventions!$A62&lt;&gt;"",interventions!$A62,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="str">
+        <f>IF(interventions!$A63&lt;&gt;"",interventions!$A63,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="str">
+        <f>IF(interventions!$A64&lt;&gt;"",interventions!$A64,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="str">
+        <f>IF(interventions!$A65&lt;&gt;"",interventions!$A65,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="str">
+        <f>IF(interventions!$A66&lt;&gt;"",interventions!$A66,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="str">
+        <f>IF(interventions!$A67&lt;&gt;"",interventions!$A67,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="str">
+        <f>IF(interventions!$A68&lt;&gt;"",interventions!$A68,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="str">
+        <f>IF(interventions!$A69&lt;&gt;"",interventions!$A69,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="str">
+        <f>IF(interventions!$A70&lt;&gt;"",interventions!$A70,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="str">
+        <f>IF(interventions!$A71&lt;&gt;"",interventions!$A71,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="str">
+        <f>IF(interventions!$A72&lt;&gt;"",interventions!$A72,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="str">
+        <f>IF(interventions!$A73&lt;&gt;"",interventions!$A73,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="str">
+        <f>IF(interventions!$A74&lt;&gt;"",interventions!$A74,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="str">
+        <f>IF(interventions!$A75&lt;&gt;"",interventions!$A75,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="str">
+        <f>IF(interventions!$A76&lt;&gt;"",interventions!$A76,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="str">
+        <f>IF(interventions!$A77&lt;&gt;"",interventions!$A77,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="str">
+        <f>IF(interventions!$A78&lt;&gt;"",interventions!$A78,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="str">
+        <f>IF(interventions!$A79&lt;&gt;"",interventions!$A79,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="str">
+        <f>IF(interventions!$A80&lt;&gt;"",interventions!$A80,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="str">
+        <f>IF(interventions!$A81&lt;&gt;"",interventions!$A81,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="str">
+        <f>IF(interventions!$A82&lt;&gt;"",interventions!$A82,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="str">
+        <f>IF(interventions!$A83&lt;&gt;"",interventions!$A83,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="str">
+        <f>IF(interventions!$A84&lt;&gt;"",interventions!$A84,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="str">
+        <f>IF(interventions!$A85&lt;&gt;"",interventions!$A85,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="str">
+        <f>IF(interventions!$A86&lt;&gt;"",interventions!$A86,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="str">
+        <f>IF(interventions!$A87&lt;&gt;"",interventions!$A87,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="str">
+        <f>IF(interventions!$A88&lt;&gt;"",interventions!$A88,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="str">
+        <f>IF(interventions!$A89&lt;&gt;"",interventions!$A89,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="str">
+        <f>IF(interventions!$A90&lt;&gt;"",interventions!$A90,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="str">
+        <f>IF(interventions!$A91&lt;&gt;"",interventions!$A91,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="str">
+        <f>IF(interventions!$A92&lt;&gt;"",interventions!$A92,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="str">
+        <f>IF(interventions!$A93&lt;&gt;"",interventions!$A93,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="str">
+        <f>IF(interventions!$A94&lt;&gt;"",interventions!$A94,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="str">
+        <f>IF(interventions!$A95&lt;&gt;"",interventions!$A95,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="str">
+        <f>IF(interventions!$A96&lt;&gt;"",interventions!$A96,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="str">
+        <f>IF(interventions!$A97&lt;&gt;"",interventions!$A97,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="str">
+        <f>IF(interventions!$A98&lt;&gt;"",interventions!$A98,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="str">
+        <f>IF(interventions!$A99&lt;&gt;"",interventions!$A99,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="str">
+        <f>IF(interventions!$A100&lt;&gt;"",interventions!$A100,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="str">
+        <f>IF(interventions!$A101&lt;&gt;"",interventions!$A101,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="str">
+        <f>IF(interventions!$A102&lt;&gt;"",interventions!$A102,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="str">
+        <f>IF(interventions!$A103&lt;&gt;"",interventions!$A103,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="str">
+        <f>IF(interventions!$A104&lt;&gt;"",interventions!$A104,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="str">
+        <f>IF(interventions!$A105&lt;&gt;"",interventions!$A105,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="str">
+        <f>IF(interventions!$A106&lt;&gt;"",interventions!$A106,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="str">
+        <f>IF(interventions!$A107&lt;&gt;"",interventions!$A107,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="str">
+        <f>IF(interventions!$A108&lt;&gt;"",interventions!$A108,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="str">
+        <f>IF(interventions!$A109&lt;&gt;"",interventions!$A109,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="str">
+        <f>IF(interventions!$A110&lt;&gt;"",interventions!$A110,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="str">
+        <f>IF(interventions!$A111&lt;&gt;"",interventions!$A111,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="str">
+        <f>IF(interventions!$A112&lt;&gt;"",interventions!$A112,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="str">
+        <f>IF(interventions!$A113&lt;&gt;"",interventions!$A113,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="str">
+        <f>IF(interventions!$A114&lt;&gt;"",interventions!$A114,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="str">
+        <f>IF(interventions!$A115&lt;&gt;"",interventions!$A115,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="str">
+        <f>IF(interventions!$A116&lt;&gt;"",interventions!$A116,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="str">
+        <f>IF(interventions!$A117&lt;&gt;"",interventions!$A117,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="str">
+        <f>IF(interventions!$A118&lt;&gt;"",interventions!$A118,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="str">
+        <f>IF(interventions!$A119&lt;&gt;"",interventions!$A119,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="str">
+        <f>IF(interventions!$A120&lt;&gt;"",interventions!$A120,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="str">
+        <f>IF(interventions!$A121&lt;&gt;"",interventions!$A121,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="str">
+        <f>IF(interventions!$A122&lt;&gt;"",interventions!$A122,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="str">
+        <f>IF(interventions!$A123&lt;&gt;"",interventions!$A123,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="str">
+        <f>IF(interventions!$A124&lt;&gt;"",interventions!$A124,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="str">
+        <f>IF(interventions!$A125&lt;&gt;"",interventions!$A125,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="str">
+        <f>IF(interventions!$A126&lt;&gt;"",interventions!$A126,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="str">
+        <f>IF(interventions!$A127&lt;&gt;"",interventions!$A127,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="str">
+        <f>IF(interventions!$A128&lt;&gt;"",interventions!$A128,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="str">
+        <f>IF(interventions!$A129&lt;&gt;"",interventions!$A129,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="str">
+        <f>IF(interventions!$A130&lt;&gt;"",interventions!$A130,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="str">
+        <f>IF(interventions!$A131&lt;&gt;"",interventions!$A131,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="str">
+        <f>IF(interventions!$A132&lt;&gt;"",interventions!$A132,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="str">
+        <f>IF(interventions!$A133&lt;&gt;"",interventions!$A133,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="str">
+        <f>IF(interventions!$A134&lt;&gt;"",interventions!$A134,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="str">
+        <f>IF(interventions!$A135&lt;&gt;"",interventions!$A135,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="str">
+        <f>IF(interventions!$A136&lt;&gt;"",interventions!$A136,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="str">
+        <f>IF(interventions!$A137&lt;&gt;"",interventions!$A137,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="str">
+        <f>IF(interventions!$A138&lt;&gt;"",interventions!$A138,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="str">
+        <f>IF(interventions!$A139&lt;&gt;"",interventions!$A139,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="str">
+        <f>IF(interventions!$A140&lt;&gt;"",interventions!$A140,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="str">
+        <f>IF(interventions!$A141&lt;&gt;"",interventions!$A141,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="str">
+        <f>IF(interventions!$A142&lt;&gt;"",interventions!$A142,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="str">
+        <f>IF(interventions!$A143&lt;&gt;"",interventions!$A143,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="str">
+        <f>IF(interventions!$A144&lt;&gt;"",interventions!$A144,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="str">
+        <f>IF(interventions!$A145&lt;&gt;"",interventions!$A145,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="str">
+        <f>IF(interventions!$A146&lt;&gt;"",interventions!$A146,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="str">
+        <f>IF(interventions!$A147&lt;&gt;"",interventions!$A147,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="str">
+        <f>IF(interventions!$A148&lt;&gt;"",interventions!$A148,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="str">
+        <f>IF(interventions!$A149&lt;&gt;"",interventions!$A149,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="str">
+        <f>IF(interventions!$A150&lt;&gt;"",interventions!$A150,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="str">
+        <f>IF(interventions!$A151&lt;&gt;"",interventions!$A151,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="str">
+        <f>IF(interventions!$A152&lt;&gt;"",interventions!$A152,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="str">
+        <f>IF(interventions!$A153&lt;&gt;"",interventions!$A153,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="str">
+        <f>IF(interventions!$A154&lt;&gt;"",interventions!$A154,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="str">
+        <f>IF(interventions!$A155&lt;&gt;"",interventions!$A155,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="str">
+        <f>IF(interventions!$A156&lt;&gt;"",interventions!$A156,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="str">
+        <f>IF(interventions!$A157&lt;&gt;"",interventions!$A157,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="str">
+        <f>IF(interventions!$A158&lt;&gt;"",interventions!$A158,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="str">
+        <f>IF(interventions!$A159&lt;&gt;"",interventions!$A159,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="str">
+        <f>IF(interventions!$A160&lt;&gt;"",interventions!$A160,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="str">
+        <f>IF(interventions!$A161&lt;&gt;"",interventions!$A161,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="str">
+        <f>IF(interventions!$A162&lt;&gt;"",interventions!$A162,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="str">
+        <f>IF(interventions!$A163&lt;&gt;"",interventions!$A163,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="str">
+        <f>IF(interventions!$A164&lt;&gt;"",interventions!$A164,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="str">
+        <f>IF(interventions!$A165&lt;&gt;"",interventions!$A165,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="str">
+        <f>IF(interventions!$A166&lt;&gt;"",interventions!$A166,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="str">
+        <f>IF(interventions!$A167&lt;&gt;"",interventions!$A167,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="str">
+        <f>IF(interventions!$A168&lt;&gt;"",interventions!$A168,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="str">
+        <f>IF(interventions!$A169&lt;&gt;"",interventions!$A169,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="str">
+        <f>IF(interventions!$A170&lt;&gt;"",interventions!$A170,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="str">
+        <f>IF(interventions!$A171&lt;&gt;"",interventions!$A171,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="str">
+        <f>IF(interventions!$A172&lt;&gt;"",interventions!$A172,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="str">
+        <f>IF(interventions!$A173&lt;&gt;"",interventions!$A173,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="str">
+        <f>IF(interventions!$A174&lt;&gt;"",interventions!$A174,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="str">
+        <f>IF(interventions!$A175&lt;&gt;"",interventions!$A175,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="str">
+        <f>IF(interventions!$A176&lt;&gt;"",interventions!$A176,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="str">
+        <f>IF(interventions!$A177&lt;&gt;"",interventions!$A177,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="str">
+        <f>IF(interventions!$A178&lt;&gt;"",interventions!$A178,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="str">
+        <f>IF(interventions!$A179&lt;&gt;"",interventions!$A179,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="str">
+        <f>IF(interventions!$A180&lt;&gt;"",interventions!$A180,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="str">
+        <f>IF(interventions!$A181&lt;&gt;"",interventions!$A181,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="str">
+        <f>IF(interventions!$A182&lt;&gt;"",interventions!$A182,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="str">
+        <f>IF(interventions!$A183&lt;&gt;"",interventions!$A183,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="str">
+        <f>IF(interventions!$A184&lt;&gt;"",interventions!$A184,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="str">
+        <f>IF(interventions!$A185&lt;&gt;"",interventions!$A185,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="str">
+        <f>IF(interventions!$A186&lt;&gt;"",interventions!$A186,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="str">
+        <f>IF(interventions!$A187&lt;&gt;"",interventions!$A187,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="str">
+        <f>IF(interventions!$A188&lt;&gt;"",interventions!$A188,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="str">
+        <f>IF(interventions!$A189&lt;&gt;"",interventions!$A189,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="str">
+        <f>IF(interventions!$A190&lt;&gt;"",interventions!$A190,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="str">
+        <f>IF(interventions!$A191&lt;&gt;"",interventions!$A191,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="str">
+        <f>IF(interventions!$A192&lt;&gt;"",interventions!$A192,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="str">
+        <f>IF(interventions!$A193&lt;&gt;"",interventions!$A193,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="str">
+        <f>IF(interventions!$A194&lt;&gt;"",interventions!$A194,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="str">
+        <f>IF(interventions!$A195&lt;&gt;"",interventions!$A195,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="str">
+        <f>IF(interventions!$A196&lt;&gt;"",interventions!$A196,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="str">
+        <f>IF(interventions!$A197&lt;&gt;"",interventions!$A197,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="str">
+        <f>IF(interventions!$A198&lt;&gt;"",interventions!$A198,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="str">
+        <f>IF(interventions!$A199&lt;&gt;"",interventions!$A199,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="str">
+        <f>IF(interventions!$A200&lt;&gt;"",interventions!$A200,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="str">
+        <f>IF(interventions!$A201&lt;&gt;"",interventions!$A201,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="str">
+        <f>IF(interventions!$A202&lt;&gt;"",interventions!$A202,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="str">
+        <f>IF(interventions!$A203&lt;&gt;"",interventions!$A203,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="str">
+        <f>IF(interventions!$A204&lt;&gt;"",interventions!$A204,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="str">
+        <f>IF(interventions!$A205&lt;&gt;"",interventions!$A205,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="str">
+        <f>IF(interventions!$A206&lt;&gt;"",interventions!$A206,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="str">
+        <f>IF(interventions!$A207&lt;&gt;"",interventions!$A207,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="str">
+        <f>IF(interventions!$A208&lt;&gt;"",interventions!$A208,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="str">
+        <f>IF(interventions!$A209&lt;&gt;"",interventions!$A209,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="str">
+        <f>IF(interventions!$A210&lt;&gt;"",interventions!$A210,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="str">
+        <f>IF(interventions!$A211&lt;&gt;"",interventions!$A211,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="str">
+        <f>IF(interventions!$A212&lt;&gt;"",interventions!$A212,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="str">
+        <f>IF(interventions!$A213&lt;&gt;"",interventions!$A213,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="str">
+        <f>IF(interventions!$A214&lt;&gt;"",interventions!$A214,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="str">
+        <f>IF(interventions!$A215&lt;&gt;"",interventions!$A215,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="str">
+        <f>IF(interventions!$A216&lt;&gt;"",interventions!$A216,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="str">
+        <f>IF(interventions!$A217&lt;&gt;"",interventions!$A217,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="str">
+        <f>IF(interventions!$A218&lt;&gt;"",interventions!$A218,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="str">
+        <f>IF(interventions!$A219&lt;&gt;"",interventions!$A219,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="str">
+        <f>IF(interventions!$A220&lt;&gt;"",interventions!$A220,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="str">
+        <f>IF(interventions!$A221&lt;&gt;"",interventions!$A221,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="str">
+        <f>IF(interventions!$A222&lt;&gt;"",interventions!$A222,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="str">
+        <f>IF(interventions!$A223&lt;&gt;"",interventions!$A223,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="str">
+        <f>IF(interventions!$A224&lt;&gt;"",interventions!$A224,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="str">
+        <f>IF(interventions!$A225&lt;&gt;"",interventions!$A225,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="str">
+        <f>IF(interventions!$A226&lt;&gt;"",interventions!$A226,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="str">
+        <f>IF(interventions!$A227&lt;&gt;"",interventions!$A227,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="str">
+        <f>IF(interventions!$A228&lt;&gt;"",interventions!$A228,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="str">
+        <f>IF(interventions!$A229&lt;&gt;"",interventions!$A229,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="str">
+        <f>IF(interventions!$A230&lt;&gt;"",interventions!$A230,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="str">
+        <f>IF(interventions!$A231&lt;&gt;"",interventions!$A231,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="str">
+        <f>IF(interventions!$A232&lt;&gt;"",interventions!$A232,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="str">
+        <f>IF(interventions!$A233&lt;&gt;"",interventions!$A233,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="str">
+        <f>IF(interventions!$A234&lt;&gt;"",interventions!$A234,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="str">
+        <f>IF(interventions!$A235&lt;&gt;"",interventions!$A235,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="str">
+        <f>IF(interventions!$A236&lt;&gt;"",interventions!$A236,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="str">
+        <f>IF(interventions!$A237&lt;&gt;"",interventions!$A237,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="str">
+        <f>IF(interventions!$A238&lt;&gt;"",interventions!$A238,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="str">
+        <f>IF(interventions!$A239&lt;&gt;"",interventions!$A239,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="str">
+        <f>IF(interventions!$A240&lt;&gt;"",interventions!$A240,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="str">
+        <f>IF(interventions!$A241&lt;&gt;"",interventions!$A241,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="str">
+        <f>IF(interventions!$A242&lt;&gt;"",interventions!$A242,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="str">
+        <f>IF(interventions!$A243&lt;&gt;"",interventions!$A243,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="str">
+        <f>IF(interventions!$A244&lt;&gt;"",interventions!$A244,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="str">
+        <f>IF(interventions!$A245&lt;&gt;"",interventions!$A245,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="str">
+        <f>IF(interventions!$A246&lt;&gt;"",interventions!$A246,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="str">
+        <f>IF(interventions!$A247&lt;&gt;"",interventions!$A247,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="str">
+        <f>IF(interventions!$A248&lt;&gt;"",interventions!$A248,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="str">
+        <f>IF(interventions!$A249&lt;&gt;"",interventions!$A249,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="str">
+        <f>IF(interventions!$A250&lt;&gt;"",interventions!$A250,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="str">
+        <f>IF(interventions!$A251&lt;&gt;"",interventions!$A251,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="str">
+        <f>IF(interventions!$A252&lt;&gt;"",interventions!$A252,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="str">
+        <f>IF(interventions!$A253&lt;&gt;"",interventions!$A253,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="str">
+        <f>IF(interventions!$A254&lt;&gt;"",interventions!$A254,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="str">
+        <f>IF(interventions!$A255&lt;&gt;"",interventions!$A255,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="str">
+        <f>IF(interventions!$A256&lt;&gt;"",interventions!$A256,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="str">
+        <f>IF(interventions!$A257&lt;&gt;"",interventions!$A257,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="str">
+        <f>IF(interventions!$A258&lt;&gt;"",interventions!$A258,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="str">
+        <f>IF(interventions!$A259&lt;&gt;"",interventions!$A259,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="str">
+        <f>IF(interventions!$A260&lt;&gt;"",interventions!$A260,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="str">
+        <f>IF(interventions!$A261&lt;&gt;"",interventions!$A261,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="str">
+        <f>IF(interventions!$A262&lt;&gt;"",interventions!$A262,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="str">
+        <f>IF(interventions!$A263&lt;&gt;"",interventions!$A263,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="str">
+        <f>IF(interventions!$A264&lt;&gt;"",interventions!$A264,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="str">
+        <f>IF(interventions!$A265&lt;&gt;"",interventions!$A265,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="str">
+        <f>IF(interventions!$A266&lt;&gt;"",interventions!$A266,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="str">
+        <f>IF(interventions!$A267&lt;&gt;"",interventions!$A267,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="str">
+        <f>IF(interventions!$A268&lt;&gt;"",interventions!$A268,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="str">
+        <f>IF(interventions!$A269&lt;&gt;"",interventions!$A269,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="str">
+        <f>IF(interventions!$A270&lt;&gt;"",interventions!$A270,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="str">
+        <f>IF(interventions!$A271&lt;&gt;"",interventions!$A271,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="str">
+        <f>IF(interventions!$A272&lt;&gt;"",interventions!$A272,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="str">
+        <f>IF(interventions!$A273&lt;&gt;"",interventions!$A273,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="str">
+        <f>IF(interventions!$A274&lt;&gt;"",interventions!$A274,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="str">
+        <f>IF(interventions!$A275&lt;&gt;"",interventions!$A275,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="str">
+        <f>IF(interventions!$A276&lt;&gt;"",interventions!$A276,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="str">
+        <f>IF(interventions!$A277&lt;&gt;"",interventions!$A277,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="str">
+        <f>IF(interventions!$A278&lt;&gt;"",interventions!$A278,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="str">
+        <f>IF(interventions!$A279&lt;&gt;"",interventions!$A279,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="str">
+        <f>IF(interventions!$A280&lt;&gt;"",interventions!$A280,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="str">
+        <f>IF(interventions!$A281&lt;&gt;"",interventions!$A281,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="str">
+        <f>IF(interventions!$A282&lt;&gt;"",interventions!$A282,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="str">
+        <f>IF(interventions!$A283&lt;&gt;"",interventions!$A283,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="str">
+        <f>IF(interventions!$A284&lt;&gt;"",interventions!$A284,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="str">
+        <f>IF(interventions!$A285&lt;&gt;"",interventions!$A285,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="2" t="str">
+        <f>IF(interventions!$A286&lt;&gt;"",interventions!$A286,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="str">
+        <f>IF(interventions!$A287&lt;&gt;"",interventions!$A287,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="2" t="str">
+        <f>IF(interventions!$A288&lt;&gt;"",interventions!$A288,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="str">
+        <f>IF(interventions!$A289&lt;&gt;"",interventions!$A289,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="str">
+        <f>IF(interventions!$A290&lt;&gt;"",interventions!$A290,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="str">
+        <f>IF(interventions!$A291&lt;&gt;"",interventions!$A291,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="str">
+        <f>IF(interventions!$A292&lt;&gt;"",interventions!$A292,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="str">
+        <f>IF(interventions!$A293&lt;&gt;"",interventions!$A293,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="2" t="str">
+        <f>IF(interventions!$A294&lt;&gt;"",interventions!$A294,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="2" t="str">
+        <f>IF(interventions!$A295&lt;&gt;"",interventions!$A295,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="str">
+        <f>IF(interventions!$A296&lt;&gt;"",interventions!$A296,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="2" t="str">
+        <f>IF(interventions!$A297&lt;&gt;"",interventions!$A297,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="str">
+        <f>IF(interventions!$A298&lt;&gt;"",interventions!$A298,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="str">
+        <f>IF(interventions!$A299&lt;&gt;"",interventions!$A299,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="str">
+        <f>IF(interventions!$A300&lt;&gt;"",interventions!$A300,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="2" t="str">
+        <f>IF(interventions!$A301&lt;&gt;"",interventions!$A301,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="2" t="str">
+        <f>IF(interventions!$A302&lt;&gt;"",interventions!$A302,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="2" t="str">
+        <f>IF(interventions!$A303&lt;&gt;"",interventions!$A303,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="2" t="str">
+        <f>IF(interventions!$A304&lt;&gt;"",interventions!$A304,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="2" t="str">
+        <f>IF(interventions!$A305&lt;&gt;"",interventions!$A305,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="str">
+        <f>IF(interventions!$A306&lt;&gt;"",interventions!$A306,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="2" t="str">
+        <f>IF(interventions!$A307&lt;&gt;"",interventions!$A307,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="2" t="str">
+        <f>IF(interventions!$A308&lt;&gt;"",interventions!$A308,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="2" t="str">
+        <f>IF(interventions!$A309&lt;&gt;"",interventions!$A309,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{F0190343-02DA-47C2-9B80-F31FDA80AF14}">
+      <formula1>"gradual, sudden"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7846C060-663F-4CB7-BA8D-E3F63239492A}">
   <sheetPr>
@@ -5877,7 +7817,7 @@
   <dimension ref="A1:KW309"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16563,8 +18503,8 @@
   </sheetPr>
   <dimension ref="A1:KW309"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>